<commit_message>
bi: update prestop forms
</commit_message>
<xml_diff>
--- a/ONCHO/Impact Assessments/Burundi/bi_oncho_prestop_1_202307_site.xlsx
+++ b/ONCHO/Impact Assessments/Burundi/bi_oncho_prestop_1_202307_site.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Impact Assessments\Burundi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C91BD20-DDCA-4FAC-B509-F15FBBB8A05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{258502F5-AE81-4E9A-8CC1-A39C65F5E956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -231,12 +231,6 @@
     <t>regex(.,'^[0-9]{2}$') and . &gt; 9 and . &lt; 1000</t>
   </si>
   <si>
-    <t>(2023 Juillet) ONCHO Stop TDM - 1. Formulaire Site V2</t>
-  </si>
-  <si>
-    <t>bj_oncho_stop_1_202306_site_v2</t>
-  </si>
-  <si>
     <t>Entrer le nom du village</t>
   </si>
   <si>
@@ -379,6 +373,12 @@
   </si>
   <si>
     <t>KIVOMA</t>
+  </si>
+  <si>
+    <t>bi_oncho_prestop_1_202307_site</t>
+  </si>
+  <si>
+    <t>(2023 Juillet) ONCHO pre Stop - 1. Formulaire Site</t>
   </si>
 </sst>
 </file>
@@ -985,7 +985,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D4" s="12"/>
       <c r="E4" s="15"/>
@@ -1009,7 +1009,7 @@
         <v>60</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D5" s="12"/>
       <c r="E5" s="15"/>
@@ -1144,7 +1144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A42" sqref="A42:XFD338"/>
     </sheetView>
@@ -1253,10 +1253,10 @@
         <v>44</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -1267,10 +1267,10 @@
         <v>44</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1281,10 +1281,10 @@
         <v>44</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -1295,10 +1295,10 @@
         <v>44</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1309,10 +1309,10 @@
         <v>44</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1323,10 +1323,10 @@
         <v>44</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1345,13 +1345,13 @@
         <v>20</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1361,13 +1361,13 @@
         <v>20</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1377,13 +1377,13 @@
         <v>20</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1393,13 +1393,13 @@
         <v>20</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1409,13 +1409,13 @@
         <v>20</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -1425,13 +1425,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -1441,13 +1441,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1457,13 +1457,13 @@
         <v>20</v>
       </c>
       <c r="B23" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -1473,13 +1473,13 @@
         <v>20</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -1489,13 +1489,13 @@
         <v>20</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -1513,14 +1513,14 @@
         <v>48</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F27" s="3"/>
     </row>
@@ -1529,14 +1529,14 @@
         <v>48</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F28" s="3"/>
     </row>
@@ -1545,14 +1545,14 @@
         <v>48</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F29" s="3"/>
     </row>
@@ -1561,14 +1561,14 @@
         <v>48</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F30" s="3"/>
     </row>
@@ -1577,14 +1577,14 @@
         <v>48</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F31" s="3"/>
     </row>
@@ -1593,14 +1593,14 @@
         <v>48</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F32" s="3"/>
     </row>
@@ -1609,14 +1609,14 @@
         <v>48</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F33" s="3"/>
     </row>
@@ -1625,14 +1625,14 @@
         <v>48</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F34" s="3"/>
     </row>
@@ -1641,14 +1641,14 @@
         <v>48</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F35" s="3"/>
     </row>
@@ -1657,14 +1657,14 @@
         <v>48</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F36" s="3"/>
     </row>
@@ -1673,14 +1673,14 @@
         <v>48</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F37" s="3"/>
     </row>
@@ -1689,14 +1689,14 @@
         <v>48</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F38" s="3"/>
     </row>
@@ -1705,14 +1705,14 @@
         <v>48</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F39" s="3"/>
     </row>
@@ -1721,14 +1721,14 @@
         <v>48</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F40" s="3"/>
     </row>
@@ -1737,14 +1737,14 @@
         <v>48</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F41" s="3"/>
     </row>
@@ -1758,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1788,10 +1788,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>63</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>111</v>
       </c>
       <c r="C2">
         <v>20201130</v>
@@ -1835,40 +1835,40 @@
   <sheetData>
     <row r="1" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="E1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="F1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>73</v>
-      </c>
       <c r="J1" s="22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="O1" s="22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P1" s="22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -1876,37 +1876,37 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="J2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="P2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1914,37 +1914,37 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="O3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="P3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1952,37 +1952,37 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G4" t="s">
+        <v>106</v>
+      </c>
+      <c r="J4" t="s">
         <v>78</v>
       </c>
-      <c r="D4" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" t="s">
-        <v>96</v>
-      </c>
-      <c r="G4" t="s">
-        <v>108</v>
-      </c>
-      <c r="J4" t="s">
-        <v>80</v>
-      </c>
       <c r="L4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="O4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="P4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1990,37 +1990,37 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="M5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -2028,37 +2028,37 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J6" t="s">
+        <v>77</v>
+      </c>
+      <c r="L6" t="s">
         <v>78</v>
       </c>
-      <c r="D6" t="s">
+      <c r="M6" t="s">
         <v>83</v>
       </c>
-      <c r="E6" t="s">
-        <v>89</v>
-      </c>
-      <c r="F6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G6" t="s">
-        <v>98</v>
-      </c>
-      <c r="J6" t="s">
-        <v>79</v>
-      </c>
-      <c r="L6" t="s">
-        <v>80</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>85</v>
       </c>
-      <c r="O6" t="s">
-        <v>87</v>
-      </c>
       <c r="P6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -2066,37 +2066,37 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J7" t="s">
         <v>80</v>
       </c>
-      <c r="D7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F7" t="s">
-        <v>99</v>
-      </c>
-      <c r="G7" t="s">
-        <v>99</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
+        <v>78</v>
+      </c>
+      <c r="M7" t="s">
         <v>82</v>
       </c>
-      <c r="L7" t="s">
-        <v>80</v>
-      </c>
-      <c r="M7" t="s">
-        <v>84</v>
-      </c>
       <c r="O7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -2104,34 +2104,34 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" t="s">
+        <v>82</v>
+      </c>
+      <c r="E8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" t="s">
+        <v>107</v>
+      </c>
+      <c r="L8" t="s">
         <v>75</v>
       </c>
-      <c r="C8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E8" t="s">
-        <v>90</v>
-      </c>
-      <c r="F8" t="s">
-        <v>100</v>
-      </c>
-      <c r="G8" t="s">
-        <v>109</v>
-      </c>
-      <c r="L8" t="s">
-        <v>77</v>
-      </c>
       <c r="M8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="O8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -2139,34 +2139,34 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G9" t="s">
+        <v>99</v>
+      </c>
+      <c r="L9" t="s">
+        <v>77</v>
+      </c>
+      <c r="M9" t="s">
         <v>75</v>
       </c>
-      <c r="C9" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" t="s">
-        <v>85</v>
-      </c>
-      <c r="E9" t="s">
-        <v>91</v>
-      </c>
-      <c r="F9" t="s">
-        <v>101</v>
-      </c>
-      <c r="G9" t="s">
-        <v>101</v>
-      </c>
-      <c r="L9" t="s">
-        <v>79</v>
-      </c>
-      <c r="M9" t="s">
-        <v>77</v>
-      </c>
       <c r="O9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -2174,34 +2174,34 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G10" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="P10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -2209,34 +2209,34 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" t="s">
+        <v>108</v>
+      </c>
+      <c r="L11" t="s">
+        <v>80</v>
+      </c>
+      <c r="M11" t="s">
+        <v>80</v>
+      </c>
+      <c r="O11" t="s">
         <v>75</v>
       </c>
-      <c r="C11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E11" t="s">
-        <v>86</v>
-      </c>
-      <c r="F11" t="s">
-        <v>102</v>
-      </c>
-      <c r="G11" t="s">
-        <v>110</v>
-      </c>
-      <c r="L11" t="s">
-        <v>82</v>
-      </c>
-      <c r="M11" t="s">
-        <v>82</v>
-      </c>
-      <c r="O11" t="s">
-        <v>77</v>
-      </c>
       <c r="P11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -2244,28 +2244,28 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D12" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -2273,28 +2273,28 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -2302,28 +2302,28 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F14" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" t="s">
+        <v>110</v>
+      </c>
+      <c r="O14" t="s">
+        <v>80</v>
+      </c>
+      <c r="P14" t="s">
         <v>104</v>
-      </c>
-      <c r="G14" t="s">
-        <v>112</v>
-      </c>
-      <c r="O14" t="s">
-        <v>82</v>
-      </c>
-      <c r="P14" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -2331,28 +2331,28 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="O15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="P15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -2360,28 +2360,28 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="O16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="P16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>